<commit_message>
updating code to pytorch 1.3 and new models for scenes of shape 200x200x50
</commit_message>
<xml_diff>
--- a/cup_generator/Arch.xlsx
+++ b/cup_generator/Arch.xlsx
@@ -475,10 +475,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:O55"/>
+  <dimension ref="B1:O56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1825,7 +1825,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="1" t="n">
-        <f aca="false">(B43-1)*E43-2*D43+C43</f>
+        <f aca="false">(B43-1)*E43-2*D43+F43*(C43-1)+1</f>
         <v>5</v>
       </c>
     </row>
@@ -1847,7 +1847,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="1" t="n">
-        <f aca="false">(B44-1)*E44-2*D44+C44</f>
+        <f aca="false">(B44-1)*E44-2*D44+F44*(C44-1)+1</f>
         <v>12</v>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="1" t="n">
-        <f aca="false">(B45-1)*E45-2*D45+C45</f>
+        <f aca="false">(B45-1)*E45-2*D45+F45*(C45-1)+1</f>
         <v>24</v>
       </c>
     </row>
@@ -1891,7 +1891,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="1" t="n">
-        <f aca="false">(B46-1)*E46-2*D46+C46</f>
+        <f aca="false">(B46-1)*E46-2*D46+F46*(C46-1)+1</f>
         <v>50</v>
       </c>
     </row>
@@ -1913,17 +1913,31 @@
         <v>1</v>
       </c>
       <c r="G47" s="1" t="n">
-        <f aca="false">(B47-1)*E47-2*D47+C47</f>
+        <f aca="false">(B47-1)*E47-2*D47+F47*(C47-1)+1</f>
         <v>100</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="0"/>
-      <c r="C48" s="0"/>
-      <c r="D48" s="0"/>
-      <c r="E48" s="0"/>
-      <c r="F48" s="0"/>
-      <c r="G48" s="0"/>
+      <c r="B48" s="1" t="n">
+        <f aca="false">G47</f>
+        <v>100</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D48" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" s="1" t="n">
+        <f aca="false">(B48-1)*E48-2*D48+F48*(C48-1)+1</f>
+        <v>200</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0"/>
@@ -1955,7 +1969,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="1" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>8</v>
@@ -1971,13 +1985,13 @@
       </c>
       <c r="G51" s="1" t="n">
         <f aca="false">ROUNDDOWN((B51+2*D51-F51*(C51-1)-1)/E51 + 1,0)</f>
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="1" t="n">
         <f aca="false">G51</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>4</v>
@@ -1986,20 +2000,20 @@
         <v>1</v>
       </c>
       <c r="E52" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G52" s="1" t="n">
         <f aca="false">ROUNDDOWN((B52+2*D52-F52*(C52-1)-1)/E52 + 1,0)</f>
-        <v>17</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="1" t="n">
         <f aca="false">G52</f>
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>4</v>
@@ -2008,20 +2022,20 @@
         <v>1</v>
       </c>
       <c r="E53" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G53" s="1" t="n">
         <f aca="false">ROUNDDOWN((B53+2*D53-F53*(C53-1)-1)/E53 + 1,0)</f>
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="1" t="n">
         <f aca="false">G53</f>
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>4</v>
@@ -2037,28 +2051,50 @@
       </c>
       <c r="G54" s="1" t="n">
         <f aca="false">ROUNDDOWN((B54+2*D54-F54*(C54-1)-1)/E54 + 1,0)</f>
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="1" t="n">
         <f aca="false">G54</f>
+        <v>12</v>
+      </c>
+      <c r="C55" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D55" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" s="1" t="n">
         <v>3</v>
-      </c>
-      <c r="C55" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D55" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E55" s="1" t="n">
-        <v>2</v>
       </c>
       <c r="F55" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G55" s="1" t="n">
         <f aca="false">ROUNDDOWN((B55+2*D55-F55*(C55-1)-1)/E55 + 1,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="1" t="n">
+        <f aca="false">G55</f>
+        <v>4</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D56" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F56" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G56" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B56+2*D56-F56*(C56-1)-1)/E56 + 1,0)</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>